<commit_message>
Updated work on CoinMetrics
</commit_message>
<xml_diff>
--- a/Provider_Coin_IDs.xlsx
+++ b/Provider_Coin_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Projects/CCAF/crypto-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF111BA4-5320-E74A-A1A6-D5C2F2EE1F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10464DF-8B55-7E4A-870C-04301FDEE770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="1540" windowWidth="23900" windowHeight="22540" xr2:uid="{AD6771D4-4A22-B645-9614-CEE089E9EA73}"/>
+    <workbookView xWindow="20440" yWindow="500" windowWidth="13300" windowHeight="20500" xr2:uid="{AD6771D4-4A22-B645-9614-CEE089E9EA73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
   <si>
     <t>Tether</t>
   </si>
@@ -74,9 +74,6 @@
     <t>TerraUSD</t>
   </si>
   <si>
-    <t>Stasis Eruo</t>
-  </si>
-  <si>
     <t>Neutrino Dollar</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>tether</t>
   </si>
   <si>
-    <t>binance-coin</t>
-  </si>
-  <si>
     <t>usd-coin</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>pax-dollar</t>
   </si>
   <si>
-    <t>trueusd</t>
-  </si>
-  <si>
     <t>gemini-dollar</t>
   </si>
   <si>
@@ -170,9 +161,6 @@
     <t>USDT</t>
   </si>
   <si>
-    <t>BNB</t>
-  </si>
-  <si>
     <t>USDC</t>
   </si>
   <si>
@@ -233,9 +221,6 @@
     <t>usdc</t>
   </si>
   <si>
-    <t>bnb_eth</t>
-  </si>
-  <si>
     <t>xdb</t>
   </si>
   <si>
@@ -282,13 +267,49 @@
   </si>
   <si>
     <t>dsd</t>
+  </si>
+  <si>
+    <t>CoinMarketCap</t>
+  </si>
+  <si>
+    <t>BUSD</t>
+  </si>
+  <si>
+    <t>CELO</t>
+  </si>
+  <si>
+    <t>CoinGecko</t>
+  </si>
+  <si>
+    <t>binancecoin</t>
+  </si>
+  <si>
+    <t>paxos-standard</t>
+  </si>
+  <si>
+    <t>true-usd</t>
+  </si>
+  <si>
+    <t>frax-share</t>
+  </si>
+  <si>
+    <t>FXS</t>
+  </si>
+  <si>
+    <t>busd</t>
+  </si>
+  <si>
+    <t>Stasis Euro</t>
+  </si>
+  <si>
+    <t>binance-usd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -309,6 +330,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Var(--jp-code-font-family)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -361,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -369,6 +401,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,335 +717,403 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314A5630-CEE5-BF40-8438-AD3EFAABC458}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
         <v>51</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E17" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
         <v>55</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>